<commit_message>
include final version of python script for generating spreadsheet
</commit_message>
<xml_diff>
--- a/Prestech_form_techs_experiences_Aron_2024-12-31.xlsx
+++ b/Prestech_form_techs_experiences_Aron_2024-12-31.xlsx
@@ -56,7 +56,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -72,19 +72,29 @@
         <color rgb="00DDDDDD"/>
       </right>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="00DDDDDD"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="00EEEEEE"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -458,12 +468,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="130.8" customWidth="1" min="1" max="1"/>
-    <col width="109.2" customWidth="1" min="2" max="2"/>
-    <col width="130.8" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="165.6" customWidth="1" min="5" max="5"/>
-    <col width="84" customWidth="1" min="6" max="6"/>
+    <col width="136.25" customWidth="1" min="1" max="1"/>
+    <col width="113.75" customWidth="1" min="2" max="2"/>
+    <col width="136.25" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="172.5" customWidth="1" min="5" max="5"/>
+    <col width="87.5" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -504,59 +514,59 @@
           <t>Planilhamento (Microsoft Excel, Google Sheets, Libre Office Calc, etc.)</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Planilhamento?</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Planilhamento?</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Fórmulas Avançadas | Tabelas Dinâmicas | Macros/VBA | Gráficos e Dashboards | Validação de Dados | Colaboração em Tempo Real</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Organizar e analisar dados de forma estruturada</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Redação de Documentos (Microsoft Word, Google Docs, Libre Office Writer, etc.)</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Redação de Documentos?</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Redação de Documentos?</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Modelos e Templates | Referências Cruzadas | Mala Direta | Estilos e Formatação Automática | Exportação para PDF</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Criar, editar e formatar documentos</t>
         </is>
@@ -568,59 +578,59 @@
           <t>Softwares de Planejamento de Recursos de Negócios (SAP, SAT, TOTVS, Salesforce, ERPGo, etc.)</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Softwares de Planejamento de Recursos de Negócios?</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Softwares de Planejamento de Recursos de Negócios?</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Gestão de Estoques | Controle Financeiro | Relatórios de Faturamento | Monitoramento de Processos | Gestão de Produção</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Gerenciar processos empresariais em áreas como finanças e logística.</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Softwares de Gerenciamento de Relação com Clientes (Monday.com, ClickUp, Slack, Jira, etc.)</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Softwares de Gerenciamento de Relação com Clientes?</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Softwares de Gerenciamento de Relação com Clientes?</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>Automação de Vendas | Gestão de Relacionamento | Relatórios de Análise | Integrações com Email | Segmentação de Clientes</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>Acompanhar funil de vendas e relacionamento com clientes.</t>
         </is>
@@ -632,59 +642,59 @@
           <t>Aplicativos de Gestão de Atividades e Planejamento (Notion, Trello, Microsoft Planner, Google Calendar, etc.)</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Aplicativos de Gestão de Atividades e Planejamento?</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Aplicativos de Gestão de Atividades e Planejamento?</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Gestão de Tarefas | Criação de Workflows | Colaboração em Tempo Real | Monitoramento de Progresso</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>Organizar tarefas, projetos e equipes de forma ágil.</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Aplicativos de Inteligência de Negócios (PowerBI, Qlik Sense, Tableau, etc.)</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Aplicativos de Inteligência de Negócios?</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Aplicativos de Inteligência de Negócios?</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>Painéis Interativos | Visualização de Dados | Integração com múltiplas fontes</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>Suportar análise de dados corporativos e tomada de decisão.</t>
         </is>
@@ -696,59 +706,59 @@
           <t>Construtores de Formulários (Google Forms, Jotform, Typeform, etc.)</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Construtores de Formulários?</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Construtores de Formulários?</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Criação de Formulários | Coleta de Respostas | Integração com planilhas</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>Facilitar pesquisa, feedback e coleta de dados.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Aplicativos de Armazenamento em Nuvem (Google Drive, Dropbox, Amazon S3, etc.)</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Aplicativos de Armazenamento em Nuvem?</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Aplicativos de Armazenamento em Nuvem?</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E9" s="5" t="inlineStr">
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>Armazenamento e Compartilhamento de Arquivos | Backup e Sincronização</t>
         </is>
       </c>
-      <c r="F9" s="5" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>Disponibilizar arquivos e dados na nuvem de forma segura.</t>
         </is>
@@ -760,59 +770,59 @@
           <t>Grande Modelos de Linguagem — LLMs (ChatGPT, GitHub Copilot, Gemini, LLaMa, etc.)</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Grande Modelos de Linguagem?</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Grande Modelos de Linguagem?</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Geração de Relatórios | Criação de Scripts e Templates | Análise e Resumo de Textos | Tradução Automática | Geração de Código</t>
         </is>
       </c>
-      <c r="F10" s="3" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>Automatizar e otimizar tarefas de redação ou análise de texto.</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>Inteligências Artificiais Generativas de Imagem (Dall-E, Midjourney, Stable Diffusion, etc.)</t>
         </is>
       </c>
-      <c r="B11" s="5" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Inteligências Artificiais Generativas de Imagem?</t>
         </is>
       </c>
-      <c r="C11" s="5" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Inteligências Artificiais Generativas de Imagem?</t>
         </is>
       </c>
-      <c r="D11" s="5" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E11" s="5" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Criação de Imagens Publicitárias | Edição de Fotos | Prototipação artística | Finalidades Artísticas Diversas</t>
         </is>
       </c>
-      <c r="F11" s="5" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Produzir imagens estáticas com base em prompts textuais.</t>
         </is>
@@ -824,27 +834,27 @@
           <t>Inteligências Artificiais Generativas de Vídeo (Sora, Runway, Fliki, etc.)</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Inteligências Artificiais Generativas de Vídeo?</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Inteligências Artificiais Generativas de Vídeo?</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>Geração de Vídeos Promocionais | Apresentações Audiovisuais | Alimentação de Conteúdos em Mídias Sociais | Finalidades Artísticas Diversas</t>
         </is>
       </c>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>Produzir ou editar vídeos com base em prompts textuais ou referências.</t>
         </is>
@@ -856,27 +866,27 @@
           <t>Inteligências Artificiais Generativas de Áudio (ElevenLabs, PlayHT, ParrotAI, etc.)</t>
         </is>
       </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="B13" s="4" t="inlineStr">
         <is>
           <t>Qual é o seu nível de familiaridade com Inteligências Artificiais Generativas de Áudio?</t>
         </is>
       </c>
-      <c r="C13" s="5" t="inlineStr">
+      <c r="C13" s="4" t="inlineStr">
         <is>
           <t>Qual é o seu nível de interesse em aprender/trabalhar com Inteligências Artificiais Generativas de Áudio?</t>
         </is>
       </c>
-      <c r="D13" s="5" t="inlineStr">
+      <c r="D13" s="4" t="inlineStr">
         <is>
           <t>0 a 5</t>
         </is>
       </c>
-      <c r="E13" s="5" t="inlineStr">
+      <c r="E13" s="4" t="inlineStr">
         <is>
           <t>Acessibilidade | Apresentações Audiovisuais | Finalidades Artísticas Diversas</t>
         </is>
       </c>
-      <c r="F13" s="5" t="inlineStr">
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>Gerar ou transformar áudio/voz de forma automatizada.</t>
         </is>
@@ -901,10 +911,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="39.6" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="33.75" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="142.8" customWidth="1" min="4" max="4"/>
+    <col width="148.75" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -935,39 +945,39 @@
           <t>Nome</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Texto</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Não aceita números ou caracteres especiais</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Sobrenome</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Texto</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Não aceita números ou caracteres especiais</t>
         </is>
@@ -979,39 +989,39 @@
           <t>Idade</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Número</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>Máximo 127 | Somente dígitos numéricos</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Gênero</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Texto</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>Masculino | Feminino | Não-binário | Outros</t>
         </is>
@@ -1023,39 +1033,39 @@
           <t>E-mail Primário</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Texto</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>Mínimo 8 caracteres | Máximo 16383 caracteres | Deve incluir @ e .</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>E-mail Secundário</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Texto</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>Mínimo 8 caracteres | Máximo 16383 caracteres | Deve incluir @ e .</t>
         </is>
@@ -1067,39 +1077,39 @@
           <t>Telefone</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Inteiro</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>Só aceita números, hífens e +</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Telefone Secundário</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Inteiro</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>Só aceita números, hífens e +</t>
         </is>
@@ -1111,17 +1121,17 @@
           <t>Cargo</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Texto</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>Executivo/Administrativo | Gerência/Direção | Supervisão | Financeiro | Compras | Suporte | Operações | Desenvolvimento</t>
         </is>
@@ -1130,20 +1140,24 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>Tempo na Empresa (em meses)Número</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr">
+          <t>Tempo na Empresa (em meses)</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Número</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="C11" s="5" t="inlineStr">
+      <c r="D11" s="4" t="inlineStr">
         <is>
           <t>Somente números</t>
         </is>
       </c>
-      <c r="D11" s="5" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>